<commit_message>
update notes of IELTS and journals
</commit_message>
<xml_diff>
--- a/Words/Synonyms/Synonyms.xlsx
+++ b/Words/Synonyms/Synonyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\Synonyms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6981F389-8C41-41A7-8602-1724E1551AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803CE1B9-0D58-48EA-BA94-0F0182BDE514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>meticulous</t>
   </si>
@@ -46,6 +46,30 @@
   </si>
   <si>
     <t>essential</t>
+  </si>
+  <si>
+    <t>evident</t>
+  </si>
+  <si>
+    <t>obvious</t>
+  </si>
+  <si>
+    <t>adj.</t>
+  </si>
+  <si>
+    <t>government  regualtion</t>
+  </si>
+  <si>
+    <t>governmental oversight</t>
+  </si>
+  <si>
+    <t>rules / regulatory requirements</t>
+  </si>
+  <si>
+    <t>detrimental (formal)</t>
+  </si>
+  <si>
+    <t>harmful / damaging</t>
   </si>
 </sst>
 </file>
@@ -69,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -92,15 +116,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -108,6 +155,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,234 +447,262 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="2"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add the journal of 16 July 2025
</commit_message>
<xml_diff>
--- a/Words/Synonyms/Synonyms.xlsx
+++ b/Words/Synonyms/Synonyms.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\Synonyms\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803CE1B9-0D58-48EA-BA94-0F0182BDE514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>meticulous</t>
   </si>
@@ -70,12 +64,24 @@
   </si>
   <si>
     <t>harmful / damaging</t>
+  </si>
+  <si>
+    <t>ambiguous</t>
+  </si>
+  <si>
+    <t>equivocal</t>
+  </si>
+  <si>
+    <t>umambiguous</t>
+  </si>
+  <si>
+    <t>unequivocal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,7 +172,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -224,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -259,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -436,18 +442,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,15 +556,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>